<commit_message>
slim thic w yo code ahh
</commit_message>
<xml_diff>
--- a/font_test.xlsx
+++ b/font_test.xlsx
@@ -536,7 +536,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>GNZG</t>
         </is>
@@ -573,9 +573,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TX</t>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>GNZG</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>STAN</t>
         </is>
@@ -812,9 +812,9 @@
           <t>Las Vegas</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>MARQ</t>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>STAN</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -839,9 +839,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>TX</t>
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>STAN</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -854,9 +854,9 @@
           <t>Austin</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>UCLA</t>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>STAN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -876,7 +876,7 @@
           <t>TX</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>ALAST</t>
         </is>
@@ -913,9 +913,9 @@
           <t>TX</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>INCAR</t>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>ALAST</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">

</xml_diff>